<commit_message>
Set free redraw based on character count
</commit_message>
<xml_diff>
--- a/Assets/Excel/heroes.xlsx
+++ b/Assets/Excel/heroes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ulko\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59448EF7-FE22-4B73-A1D2-2C42F6D1A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B06CF74-7EBF-4B93-B94B-7C11AD101F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15315" yWindow="3780" windowWidth="17460" windowHeight="15345" activeTab="4" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="heroes" sheetId="1" r:id="rId1"/>
@@ -1880,7 +1880,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,16 +1927,16 @@
       </c>
       <c r="D2" s="2">
         <f>50-E2-F2-G2</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>12</v>
       </c>
       <c r="F2" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>